<commit_message>
working script -- adding verifying_chat_opened
</commit_message>
<xml_diff>
--- a/whatsapp_sent_log.xlsx
+++ b/whatsapp_sent_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,58 +458,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SEOANE NAHUEL</t>
+          <t>ROMERO GUSTAVO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+5491133983542</t>
+          <t>+5491544735404</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>344088.35</v>
+        <v>41000</v>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>Sent</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CANFORA TOMAS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+5491153125728</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>99999</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sent</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DEFEIS KARINA</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>+5491549867663</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>25000</v>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>Sent</t>
         </is>

</xml_diff>